<commit_message>
Finalizando proyecto agregandole el authorization y el thunder
</commit_message>
<xml_diff>
--- a/src/company/reporte_empresas.xlsx
+++ b/src/company/reporte_empresas.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Nombre</t>
   </si>
@@ -31,58 +31,40 @@
     <t>CEO</t>
   </si>
   <si>
-    <t>ArteDol</t>
-  </si>
-  <si>
-    <t>Manualidades</t>
-  </si>
-  <si>
-    <t>nacional</t>
-  </si>
-  <si>
-    <t>Artesanias</t>
+    <t>Mc</t>
+  </si>
+  <si>
+    <t>Industria de las hamburguesas</t>
+  </si>
+  <si>
+    <t>Mundial</t>
+  </si>
+  <si>
+    <t>Comida Rapida</t>
   </si>
   <si>
     <t>Rudgar Leiva</t>
   </si>
   <si>
-    <t>Mc</t>
-  </si>
-  <si>
-    <t>Industria de hamburguesas</t>
-  </si>
-  <si>
-    <t>Mundial</t>
-  </si>
-  <si>
-    <t>Comida rapida</t>
-  </si>
-  <si>
-    <t>Jhon Ramirez</t>
-  </si>
-  <si>
-    <t>Bk</t>
+    <t>BK</t>
   </si>
   <si>
     <t>Hamburguesas</t>
   </si>
   <si>
-    <t>Pedro Hernandez</t>
+    <t>Pedro</t>
   </si>
   <si>
     <t>Zara</t>
   </si>
   <si>
-    <t>Ropa</t>
+    <t>Venta de ropa</t>
   </si>
   <si>
     <t>Moda</t>
   </si>
   <si>
-    <t>Taco bell</t>
-  </si>
-  <si>
-    <t>Burritos</t>
+    <t>Juan</t>
   </si>
 </sst>
 </file>
@@ -459,7 +441,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
@@ -517,76 +499,56 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
         <v>13</v>
-      </c>
-      <c r="D3">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="F4" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
       <c r="F5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>